<commit_message>
feat: Add Correlation-Based Multivariate Stress Testing
- Add compute_covariance_matrix and run_multivariate_stress_test to RiskEngine
- Simulate Normal vs Panic (corr=0.9) regimes using Cholesky decomposition
- Aggregate asset returns from current holdings for correlation analysis
- Display new stress test table in dashboard with 20-Day VaR/CVaR
- Fix VaR chart title to clarify 'Daily 95% VaR (1-Year Lookback)'
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathanku\Documents\Jonathan Ku\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathanku\Documents\Jonathan Ku\Code\portfolio-analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515E7550-0AB5-4BE5-808F-DAF430B07B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C968B7C6-9673-48B5-B368-3EFB30CA898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8EA60FCF-4346-4BFB-9BDD-5C3F6E9B800C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="75">
   <si>
     <t>1590 TT Equity</t>
   </si>
@@ -272,6 +272,12 @@
   <si>
     <t>Short Realtek as don’t see any fundamental change on the supply side but stock price goes up too much. Still see consumer electronic demand weakness due to price hikes.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMD US Equity</t>
+  </si>
+  <si>
+    <t>AMZN US Equity</t>
   </si>
 </sst>
 </file>
@@ -671,10 +677,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CE1F1C-6449-4823-8862-D52CEA75E8AA}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3108,7 +3114,7 @@
         <v>-4000</v>
       </c>
       <c r="D173" s="4">
-        <v>48647.05</v>
+        <v>48694.400000000001</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -3140,6 +3146,48 @@
         <v>55781</v>
       </c>
       <c r="F175" s="4"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="3">
+        <v>46044</v>
+      </c>
+      <c r="B176" t="s">
+        <v>49</v>
+      </c>
+      <c r="C176">
+        <v>-400</v>
+      </c>
+      <c r="D176" s="4">
+        <v>70534.759999999995</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="3">
+        <v>46044</v>
+      </c>
+      <c r="B177" t="s">
+        <v>73</v>
+      </c>
+      <c r="C177">
+        <v>200</v>
+      </c>
+      <c r="D177" s="4">
+        <v>-50490.54</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="3">
+        <v>46044</v>
+      </c>
+      <c r="B178" t="s">
+        <v>74</v>
+      </c>
+      <c r="C178">
+        <v>300</v>
+      </c>
+      <c r="D178" s="4">
+        <v>-70207.02</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat: Add real local price support for Holdings and Trade Price for trades
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathanku\Documents\Jonathan Ku\Code\portfolio-analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C968B7C6-9673-48B5-B368-3EFB30CA898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42542518-CE25-4910-B098-26F51E9DB263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8EA60FCF-4346-4BFB-9BDD-5C3F6E9B800C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8EA60FCF-4346-4BFB-9BDD-5C3F6E9B800C}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="76">
   <si>
     <t>1590 TT Equity</t>
   </si>
@@ -278,6 +278,10 @@
   </si>
   <si>
     <t>AMZN US Equity</t>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -679,8 +683,8 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -705,6 +709,9 @@
       <c r="D1" t="s">
         <v>66</v>
       </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -719,7 +726,9 @@
       <c r="D2" s="4">
         <v>-120109.2</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5">
+        <v>899.01869999999997</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -734,6 +743,9 @@
       <c r="D3" s="4">
         <v>-212422.32</v>
       </c>
+      <c r="E3">
+        <v>383.74799999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -748,6 +760,9 @@
       <c r="D4" s="4">
         <v>122479.9</v>
       </c>
+      <c r="E4">
+        <v>215.70769999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -762,6 +777,9 @@
       <c r="D5" s="4">
         <v>213452.09</v>
       </c>
+      <c r="E5">
+        <v>13340.7554</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -776,6 +794,9 @@
       <c r="D6" s="4">
         <v>-218724.07</v>
       </c>
+      <c r="E6">
+        <v>13670.254499999999</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -790,6 +811,9 @@
       <c r="D7" s="4">
         <v>215803.35</v>
       </c>
+      <c r="E7">
+        <v>13487.7094</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -804,6 +828,9 @@
       <c r="D8" s="4">
         <v>-331704.09999999998</v>
       </c>
+      <c r="E8">
+        <v>105.7239</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -818,6 +845,9 @@
       <c r="D9" s="4">
         <v>341809.6</v>
       </c>
+      <c r="E9">
+        <v>2478.4602</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -832,6 +862,9 @@
       <c r="D10" s="4">
         <v>-250051.20000000001</v>
       </c>
+      <c r="E10">
+        <v>450.60849999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -846,6 +879,9 @@
       <c r="D11" s="4">
         <v>250608</v>
       </c>
+      <c r="E11">
+        <v>62.832799999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -860,6 +896,9 @@
       <c r="D12" s="4">
         <v>-261513</v>
       </c>
+      <c r="E12">
+        <v>765.63260000000002</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -874,6 +913,9 @@
       <c r="D13" s="4">
         <v>115447.2</v>
       </c>
+      <c r="E13">
+        <v>844.98720000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -888,6 +930,9 @@
       <c r="D14" s="4">
         <v>141680</v>
       </c>
+      <c r="E14">
+        <v>11.8527</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -902,6 +947,9 @@
       <c r="D15" s="4">
         <v>248275.5</v>
       </c>
+      <c r="E15">
+        <v>132.16040000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -916,8 +964,11 @@
       <c r="D16" s="4">
         <v>-247526</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>63.015000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45861</v>
       </c>
@@ -930,8 +981,11 @@
       <c r="D17" s="4">
         <v>-125742.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>216.9933</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45861</v>
       </c>
@@ -944,8 +998,11 @@
       <c r="D18" s="4">
         <v>131604</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>11.698700000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45867</v>
       </c>
@@ -958,8 +1015,11 @@
       <c r="D19" s="4">
         <v>-223735.37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>13983.460499999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45867</v>
       </c>
@@ -972,8 +1032,11 @@
       <c r="D20" s="4">
         <v>223746.47</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>13984.1546</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45870</v>
       </c>
@@ -986,8 +1049,11 @@
       <c r="D21" s="4">
         <v>229856.54</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>425.93950000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45873</v>
       </c>
@@ -1000,8 +1066,11 @@
       <c r="D22" s="4">
         <v>-229906.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1915.8842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45880</v>
       </c>
@@ -1014,8 +1083,11 @@
       <c r="D23" s="4">
         <v>317806.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>288.11470000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45881</v>
       </c>
@@ -1028,8 +1100,11 @@
       <c r="D24" s="4">
         <v>128572.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>642.83889999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45881</v>
       </c>
@@ -1042,8 +1117,11 @@
       <c r="D25" s="4">
         <v>191310.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>139.9794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45881</v>
       </c>
@@ -1056,8 +1134,11 @@
       <c r="D26" s="4">
         <v>-192827.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>141.08779999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45881</v>
       </c>
@@ -1070,8 +1151,11 @@
       <c r="D27" s="4">
         <v>-175328</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>262.98390000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45881</v>
       </c>
@@ -1084,8 +1168,11 @@
       <c r="D28" s="4">
         <v>240032.03</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>2000.2669000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45881</v>
       </c>
@@ -1098,8 +1185,11 @@
       <c r="D29" s="4">
         <v>-433210.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>3248.9724000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45883</v>
       </c>
@@ -1112,8 +1202,11 @@
       <c r="D30" s="4">
         <v>-181499.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>1360.7007000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45883</v>
       </c>
@@ -1126,8 +1219,11 @@
       <c r="D31" s="4">
         <v>89279.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>669.32809999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45883</v>
       </c>
@@ -1140,8 +1236,11 @@
       <c r="D32" s="4">
         <v>87490.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>154.33410000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45883</v>
       </c>
@@ -1154,8 +1253,11 @@
       <c r="D33" s="4">
         <v>-145199.20000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>1088.5596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45883</v>
       </c>
@@ -1168,8 +1270,11 @@
       <c r="D34" s="4">
         <v>138159.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>1035.7816</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45883</v>
       </c>
@@ -1182,8 +1287,11 @@
       <c r="D35" s="4">
         <v>233365</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>636.19449999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45883</v>
       </c>
@@ -1196,8 +1304,11 @@
       <c r="D36" s="4">
         <v>-228341.53</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>14271.3457</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45888</v>
       </c>
@@ -1210,8 +1321,11 @@
       <c r="D37" s="4">
         <v>-155384.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>389.91180000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45888</v>
       </c>
@@ -1224,8 +1338,11 @@
       <c r="D38" s="4">
         <v>133626.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>670.62750000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45888</v>
       </c>
@@ -1238,8 +1355,11 @@
       <c r="D39" s="4">
         <v>-107025</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>1074.2444</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45888</v>
       </c>
@@ -1252,8 +1372,11 @@
       <c r="D40" s="4">
         <v>-204009.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>1228.6265000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45888</v>
       </c>
@@ -1266,8 +1389,11 @@
       <c r="D41" s="4">
         <v>204494.4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>1026.2879</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45888</v>
       </c>
@@ -1280,8 +1406,11 @@
       <c r="D42" s="4">
         <v>132521.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>128.7261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45888</v>
       </c>
@@ -1294,8 +1423,11 @@
       <c r="D43" s="4">
         <v>44187.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>42.921199999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45902</v>
       </c>
@@ -1308,8 +1440,11 @@
       <c r="D44" s="4">
         <v>161690.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>150.4879</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45911</v>
       </c>
@@ -1322,8 +1457,11 @@
       <c r="D45" s="4">
         <v>-167595.29999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>163.95570000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45911</v>
       </c>
@@ -1336,8 +1474,11 @@
       <c r="D46" s="4">
         <v>166257</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>64.641499999999994</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45911</v>
       </c>
@@ -1350,8 +1491,11 @@
       <c r="D47" s="4">
         <v>-43214</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>42.277000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45917</v>
       </c>
@@ -1364,8 +1508,11 @@
       <c r="D48" s="4">
         <v>-162913.29999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>168.8116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45917</v>
       </c>
@@ -1378,8 +1525,11 @@
       <c r="D49" s="4">
         <v>161374</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>242.4649</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45918</v>
       </c>
@@ -1392,8 +1542,11 @@
       <c r="D50" s="4">
         <v>231124.6</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>993.1748</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45918</v>
       </c>
@@ -1406,8 +1559,11 @@
       <c r="D51" s="4">
         <v>-232092</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>166.2209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45937</v>
       </c>
@@ -1420,8 +1576,11 @@
       <c r="D52" s="4">
         <v>144962.6</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>2210.4625999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45937</v>
       </c>
@@ -1434,8 +1593,11 @@
       <c r="D53" s="4">
         <v>-162276.79999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>309.31110000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45943</v>
       </c>
@@ -1448,8 +1610,11 @@
       <c r="D54" s="4">
         <v>142540.79999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>364.64249999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45943</v>
       </c>
@@ -1462,8 +1627,11 @@
       <c r="D55" s="4">
         <v>-98339.1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>1006.2717</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45943</v>
       </c>
@@ -1476,8 +1644,11 @@
       <c r="D56" s="4">
         <v>-109734.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>1684.3197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45943</v>
       </c>
@@ -1490,8 +1661,11 @@
       <c r="D57" s="4">
         <v>-94634</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>145.25489999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45943</v>
       </c>
@@ -1504,8 +1678,11 @@
       <c r="D58" s="4">
         <v>206589.6</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>150.9974</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45943</v>
       </c>
@@ -1518,8 +1695,11 @@
       <c r="D59" s="4">
         <v>-139937.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>859.15949999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45943</v>
       </c>
@@ -1532,8 +1712,11 @@
       <c r="D60" s="4">
         <v>94931</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>291.41860000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45951</v>
       </c>
@@ -1546,8 +1729,11 @@
       <c r="D61" s="4">
         <v>86110.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>1320.1225999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45951</v>
       </c>
@@ -1560,8 +1746,11 @@
       <c r="D62" s="4">
         <v>-209638</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>1285.5431000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45951</v>
       </c>
@@ -1574,8 +1763,11 @@
       <c r="D63" s="4">
         <v>114692</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>1758.2864999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45952</v>
       </c>
@@ -1588,8 +1780,11 @@
       <c r="D64" s="4">
         <v>98590.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>1010.2243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45952</v>
       </c>
@@ -1602,8 +1797,11 @@
       <c r="D65" s="4">
         <v>75116.600000000006</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>177.62260000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45952</v>
       </c>
@@ -1616,8 +1814,11 @@
       <c r="D66" s="4">
         <v>-174540.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>206.35939999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45953</v>
       </c>
@@ -1630,8 +1831,11 @@
       <c r="D67" s="4">
         <v>79795.600000000006</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>2456.9056</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45953</v>
       </c>
@@ -1644,8 +1848,11 @@
       <c r="D68" s="4">
         <v>-79645.440000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>2896.0617999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45957</v>
       </c>
@@ -1658,8 +1865,11 @@
       <c r="D69" s="4">
         <v>-123398.1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>541.52250000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45957</v>
       </c>
@@ -1672,8 +1882,11 @@
       <c r="D70" s="4">
         <v>162979.20000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>2503.2788</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45959</v>
       </c>
@@ -1686,8 +1899,11 @@
       <c r="D71" s="4">
         <v>84047.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>1285.9276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45959</v>
       </c>
@@ -1700,8 +1916,11 @@
       <c r="D72" s="4">
         <v>-79338.25</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>4832.6541999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45965</v>
       </c>
@@ -1714,8 +1933,11 @@
       <c r="D73" s="4">
         <v>110612.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>487.94490000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45965</v>
       </c>
@@ -1728,8 +1950,11 @@
       <c r="D74" s="4">
         <v>-95427.8</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>1473.3572999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45965</v>
       </c>
@@ -1742,8 +1967,11 @@
       <c r="D75" s="4">
         <v>102905.4</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>244.4307</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45965</v>
       </c>
@@ -1756,8 +1984,11 @@
       <c r="D76" s="4">
         <v>-61368.4</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>947.49800000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45971</v>
       </c>
@@ -1770,8 +2001,11 @@
       <c r="D77" s="4">
         <v>89540</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>138.64949999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45971</v>
       </c>
@@ -1784,8 +2018,11 @@
       <c r="D78" s="4">
         <v>-274877.2</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>4256.3347000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45971</v>
       </c>
@@ -1798,8 +2035,11 @@
       <c r="D79" s="4">
         <v>97009.9</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>231.09889999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45971</v>
       </c>
@@ -1812,8 +2052,11 @@
       <c r="D80" s="4">
         <v>88250.82</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>3235.0234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45972</v>
       </c>
@@ -1826,8 +2069,11 @@
       <c r="D81" s="4">
         <v>56063.199999999997</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>217.3853</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45972</v>
       </c>
@@ -1840,8 +2086,11 @@
       <c r="D82" s="4">
         <v>66206.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>228.1917</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45972</v>
       </c>
@@ -1854,8 +2103,11 @@
       <c r="D83" s="4">
         <v>-100094.68</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>585.4538</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45978</v>
       </c>
@@ -1868,8 +2120,11 @@
       <c r="D84" s="4">
         <v>-87372.4</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>1361.4794999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45978</v>
       </c>
@@ -1882,8 +2137,11 @@
       <c r="D85" s="4">
         <v>82206.75</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>5102.0756000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45978</v>
       </c>
@@ -1896,8 +2154,11 @@
       <c r="D86" s="4">
         <v>-163065.04</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>595819.27560000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45978</v>
       </c>
@@ -1910,8 +2171,11 @@
       <c r="D87" s="4">
         <v>91504.99</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>15250.832</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45978</v>
       </c>
@@ -1924,8 +2188,11 @@
       <c r="D88" s="4">
         <v>179141.43</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>2239.2678999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45979</v>
       </c>
@@ -1938,8 +2205,11 @@
       <c r="D89" s="4">
         <v>-153578.4</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>1597.4204</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45979</v>
       </c>
@@ -1952,8 +2222,11 @@
       <c r="D90" s="4">
         <v>130370</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>203.40309999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45979</v>
       </c>
@@ -1966,8 +2239,11 @@
       <c r="D91" s="4">
         <v>-264732</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>137.67830000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45979</v>
       </c>
@@ -1980,8 +2256,11 @@
       <c r="D92" s="4">
         <v>206944.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>922.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45979</v>
       </c>
@@ -1994,8 +2273,11 @@
       <c r="D93" s="4">
         <v>58663.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>122.0369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45979</v>
       </c>
@@ -2008,8 +2290,11 @@
       <c r="D94" s="4">
         <v>73780.800000000003</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>575.56299999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45980</v>
       </c>
@@ -2022,8 +2307,11 @@
       <c r="D95" s="4">
         <v>-198952.6</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>6213.0920999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45980</v>
       </c>
@@ -2036,8 +2324,11 @@
       <c r="D96" s="4">
         <v>134018</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>209.2637</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45980</v>
       </c>
@@ -2050,8 +2341,11 @@
       <c r="D97" s="4">
         <v>76122.78</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>558950.53130000003</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45980</v>
       </c>
@@ -2064,8 +2358,11 @@
       <c r="D98" s="4">
         <v>-148170.85</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>296.3417</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45980</v>
       </c>
@@ -2078,8 +2375,11 @@
       <c r="D99" s="4">
         <v>94184.35</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>553.1635</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45980</v>
       </c>
@@ -2092,8 +2392,11 @@
       <c r="D100" s="4">
         <v>-161272.79999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>64.567899999999995</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45980</v>
       </c>
@@ -2106,8 +2409,11 @@
       <c r="D101" s="4">
         <v>95283.44</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>34.029800000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45980</v>
       </c>
@@ -2120,8 +2426,11 @@
       <c r="D102" s="4">
         <v>84285.88</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>119.8839</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45982</v>
       </c>
@@ -2134,8 +2443,11 @@
       <c r="D103" s="4">
         <v>299889.09999999998</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>1346.2013999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45985</v>
       </c>
@@ -2148,8 +2460,11 @@
       <c r="D104" s="4">
         <v>-31658.32</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>316.58319999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45985</v>
       </c>
@@ -2162,8 +2477,11 @@
       <c r="D105" s="4">
         <v>-90610.65</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>181.22130000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45986</v>
       </c>
@@ -2176,8 +2494,11 @@
       <c r="D106" s="4">
         <v>78951.199999999997</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>1241.4686999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45986</v>
       </c>
@@ -2190,8 +2511,11 @@
       <c r="D107" s="4">
         <v>144863.4</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>1518.6017999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45986</v>
       </c>
@@ -2204,8 +2528,11 @@
       <c r="D108" s="4">
         <v>-104645.64</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>174.40940000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45987</v>
       </c>
@@ -2218,8 +2545,11 @@
       <c r="D109" s="4">
         <v>-70103.399999999994</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>514885.0061</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45987</v>
       </c>
@@ -2232,8 +2562,11 @@
       <c r="D110" s="4">
         <v>-124472.6</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>278.76490000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45987</v>
       </c>
@@ -2246,8 +2579,11 @@
       <c r="D111" s="4">
         <v>119307.5</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <v>287.75040000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45987</v>
       </c>
@@ -2260,8 +2596,11 @@
       <c r="D112" s="4">
         <v>-90211.34</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <v>15035.223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45987</v>
       </c>
@@ -2274,8 +2613,11 @@
       <c r="D113" s="4">
         <v>90130.75</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <v>15021.792299999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45987</v>
       </c>
@@ -2288,8 +2630,11 @@
       <c r="D114" s="4">
         <v>-176832.32</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <v>2210.404</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>45988</v>
       </c>
@@ -2302,8 +2647,11 @@
       <c r="D115" s="4">
         <v>-88961.4</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <v>1394.2906</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>45988</v>
       </c>
@@ -2316,8 +2664,11 @@
       <c r="D116" s="4">
         <v>-86390.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116">
+        <v>2707.9951000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45988</v>
       </c>
@@ -2330,8 +2681,11 @@
       <c r="D117" s="4">
         <v>-53665.8</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <v>280.36860000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45988</v>
       </c>
@@ -2344,8 +2698,11 @@
       <c r="D118" s="4">
         <v>82455</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <v>516.92669999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45988</v>
       </c>
@@ -2358,8 +2715,11 @@
       <c r="D119" s="4">
         <v>91888</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>288.03289999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45989</v>
       </c>
@@ -2372,8 +2732,11 @@
       <c r="D120" s="4">
         <v>52874.12</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <v>131.6095</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45989</v>
       </c>
@@ -2386,8 +2749,11 @@
       <c r="D121" s="4">
         <v>-83454.399999999994</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>1309.8580999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45989</v>
       </c>
@@ -2400,8 +2766,11 @@
       <c r="D122" s="4">
         <v>-81768</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <v>1283.3901000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45989</v>
       </c>
@@ -2414,8 +2783,11 @@
       <c r="D123" s="4">
         <v>-140322.70000000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123">
+        <v>629.26670000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45989</v>
       </c>
@@ -2428,8 +2800,11 @@
       <c r="D124" s="4">
         <v>163699.20000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124">
+        <v>142.74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45989</v>
       </c>
@@ -2442,8 +2817,11 @@
       <c r="D125" s="4">
         <v>146066.44</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>535866.69499999995</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45992</v>
       </c>
@@ -2456,8 +2834,11 @@
       <c r="D126" s="4">
         <v>-47754</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126">
+        <v>166.76179999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45992</v>
       </c>
@@ -2470,8 +2851,11 @@
       <c r="D127" s="4">
         <v>108340.8</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>141.8768</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45992</v>
       </c>
@@ -2484,8 +2868,11 @@
       <c r="D128" s="4">
         <v>-65547.600000000006</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128">
+        <v>1030.0483999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45993</v>
       </c>
@@ -2498,8 +2885,11 @@
       <c r="D129" s="4">
         <v>-15815.1</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129">
+        <v>165.5164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45993</v>
       </c>
@@ -2512,8 +2902,11 @@
       <c r="D130" s="4">
         <v>81022.100000000006</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130">
+        <v>2543.8512000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45993</v>
       </c>
@@ -2526,8 +2919,11 @@
       <c r="D131" s="4">
         <v>-66881.8</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131">
+        <v>1049.944</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45993</v>
       </c>
@@ -2540,8 +2936,11 @@
       <c r="D132" s="4">
         <v>-64651.3</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132">
+        <v>289.9787</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45993</v>
       </c>
@@ -2554,8 +2953,11 @@
       <c r="D133" s="4">
         <v>68471.600000000006</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133">
+        <v>537.45209999999997</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>45994</v>
       </c>
@@ -2568,8 +2970,11 @@
       <c r="D134" s="4">
         <v>79474.8</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>1244.4575</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>45994</v>
       </c>
@@ -2582,8 +2987,11 @@
       <c r="D135" s="4">
         <v>19025</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135">
+        <v>595.80669999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>45995</v>
       </c>
@@ -2596,8 +3004,11 @@
       <c r="D136" s="4">
         <v>-90307.87</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136">
+        <v>15051.312099999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>46001</v>
       </c>
@@ -2610,8 +3021,11 @@
       <c r="D137" s="4">
         <v>-65917.88</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137">
+        <v>164.79470000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>46002</v>
       </c>
@@ -2624,8 +3038,11 @@
       <c r="D138" s="4">
         <v>-49113.8</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138">
+        <v>1535.4459999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>46010</v>
       </c>
@@ -2638,8 +3055,11 @@
       <c r="D139" s="4">
         <v>-49513.2</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>781.36900000000003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>46010</v>
       </c>
@@ -2652,8 +3072,11 @@
       <c r="D140" s="4">
         <v>-56781.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140">
+        <v>597.3827</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>46010</v>
       </c>
@@ -2666,8 +3089,11 @@
       <c r="D141" s="4">
         <v>135180.6</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>4266.5690999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>46010</v>
       </c>
@@ -2680,8 +3106,11 @@
       <c r="D142" s="4">
         <v>-112043.1</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142">
+        <v>1178.768</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>46013</v>
       </c>
@@ -2694,8 +3123,11 @@
       <c r="D143" s="4">
         <v>-89220.3</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>938.0607</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>46013</v>
       </c>
@@ -2708,8 +3140,11 @@
       <c r="D144" s="4">
         <v>-104762.3</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144">
+        <v>3304.4110999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>46013</v>
       </c>
@@ -2722,8 +3157,11 @@
       <c r="D145" s="4">
         <v>135389.5</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145">
+        <v>4270.4548999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>46017</v>
       </c>
@@ -2736,8 +3174,11 @@
       <c r="D146" s="4">
         <v>-94030.399999999994</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>173.8682</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>46017</v>
       </c>
@@ -2750,8 +3191,11 @@
       <c r="D147" s="4">
         <v>-92910</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147">
+        <v>146.0258</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>46017</v>
       </c>
@@ -2764,8 +3208,11 @@
       <c r="D148" s="4">
         <v>189005.76</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148">
+        <v>315.00959999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>46027</v>
       </c>
@@ -2778,8 +3225,11 @@
       <c r="D149" s="4">
         <v>-52862.400000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149">
+        <v>1664.7439999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>46027</v>
       </c>
@@ -2792,8 +3242,11 @@
       <c r="D150" s="4">
         <v>-100224</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150">
+        <v>394.53210000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>46027</v>
       </c>
@@ -2806,8 +3259,11 @@
       <c r="D151" s="4">
         <v>60628.2</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151">
+        <v>636.43589999999995</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>46027</v>
       </c>
@@ -2820,8 +3276,11 @@
       <c r="D152" s="4">
         <v>-64213</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152">
+        <v>1011.0972</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>46027</v>
       </c>
@@ -2834,8 +3293,11 @@
       <c r="D153" s="4">
         <v>67064.399999999994</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153">
+        <v>176.0008</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>46027</v>
       </c>
@@ -2848,8 +3310,11 @@
       <c r="D154" s="4">
         <v>45999.4</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154">
+        <v>1448.6133</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>46027</v>
       </c>
@@ -2862,8 +3327,11 @@
       <c r="D155" s="4">
         <v>31083</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155">
+        <v>195.7747</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>46027</v>
       </c>
@@ -2876,8 +3344,11 @@
       <c r="D156" s="4">
         <v>-99015</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>13.5585</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>46027</v>
       </c>
@@ -2890,8 +3361,11 @@
       <c r="D157" s="4">
         <v>105046.8</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157">
+        <v>551.35500000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>46028</v>
       </c>
@@ -2904,8 +3378,11 @@
       <c r="D158" s="4">
         <v>-78392.899999999994</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158">
+        <v>2468.2795999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>46028</v>
       </c>
@@ -2918,8 +3395,11 @@
       <c r="D159" s="4">
         <v>80883.199999999997</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159">
+        <v>1273.3429000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>46028</v>
       </c>
@@ -2931,6 +3411,9 @@
       </c>
       <c r="D160" s="4">
         <v>77764.800000000003</v>
+      </c>
+      <c r="E160">
+        <v>204.04259999999999</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,6 +3429,9 @@
       <c r="D161" s="4">
         <v>61752.9</v>
       </c>
+      <c r="E161">
+        <v>648.1576</v>
+      </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
@@ -2960,6 +3446,9 @@
       <c r="D162" s="4">
         <v>44319.4</v>
       </c>
+      <c r="E162">
+        <v>1395.53</v>
+      </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
@@ -2974,6 +3463,9 @@
       <c r="D163" s="4">
         <v>-81350</v>
       </c>
+      <c r="E163">
+        <v>256.15379999999999</v>
+      </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
@@ -2988,6 +3480,9 @@
       <c r="D164" s="4">
         <v>76284</v>
       </c>
+      <c r="E164">
+        <v>2413.5506</v>
+      </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
@@ -3002,6 +3497,9 @@
       <c r="D165" s="4">
         <v>-66257.2</v>
       </c>
+      <c r="E165">
+        <v>1048.1550999999999</v>
+      </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
@@ -3016,6 +3514,9 @@
       <c r="D166" s="4">
         <v>-61513.8</v>
       </c>
+      <c r="E166">
+        <v>973.11620000000005</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
@@ -3030,6 +3531,9 @@
       <c r="D167" s="4">
         <v>91666</v>
       </c>
+      <c r="E167">
+        <v>145.0103</v>
+      </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
@@ -3044,6 +3548,9 @@
       <c r="D168" s="4">
         <v>-20335.2</v>
       </c>
+      <c r="E168">
+        <v>160.8468</v>
+      </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
@@ -3058,6 +3565,9 @@
       <c r="D169" s="4">
         <v>-21107.9</v>
       </c>
+      <c r="E169">
+        <v>667.83339999999998</v>
+      </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
@@ -3072,6 +3582,9 @@
       <c r="D170" s="4">
         <v>152633.70000000001</v>
       </c>
+      <c r="E170">
+        <v>536.1508</v>
+      </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
@@ -3086,6 +3599,9 @@
       <c r="D171" s="4">
         <v>37716.800000000003</v>
       </c>
+      <c r="E171">
+        <v>1192.2661000000001</v>
+      </c>
       <c r="F171" s="4"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -3101,6 +3617,9 @@
       <c r="D172" s="4">
         <v>-36476</v>
       </c>
+      <c r="E172">
+        <v>288.2604</v>
+      </c>
       <c r="F172" s="4"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -3116,6 +3635,9 @@
       <c r="D173" s="4">
         <v>48694.400000000001</v>
       </c>
+      <c r="E173">
+        <v>385.19740000000002</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
@@ -3130,6 +3652,9 @@
       <c r="D174" s="4">
         <v>-49342.15</v>
       </c>
+      <c r="E174">
+        <v>15606.9139</v>
+      </c>
       <c r="F174" s="4"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -3145,6 +3670,9 @@
       <c r="D175" s="4">
         <v>55781</v>
       </c>
+      <c r="E175">
+        <v>16.0563</v>
+      </c>
       <c r="F175" s="4"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -3160,8 +3688,11 @@
       <c r="D176" s="4">
         <v>70534.759999999995</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176">
+        <v>176.33699999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>46044</v>
       </c>
@@ -3174,8 +3705,11 @@
       <c r="D177" s="4">
         <v>-50490.54</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177">
+        <v>252.44980000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>46044</v>
       </c>
@@ -3187,6 +3721,9 @@
       </c>
       <c r="D178" s="4">
         <v>-70207.02</v>
+      </c>
+      <c r="E178">
+        <v>234.02430000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>